<commit_message>
added some extensions and code
</commit_message>
<xml_diff>
--- a/ExampleIG/output/all-profiles.xlsx
+++ b/ExampleIG/output/all-profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="316">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-02T22:24:37+01:00</t>
+    <t>2023-11-02T22:29:48+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -906,16 +906,19 @@
     <t>http://hl7.org/fhir/ValueSet/link-type|4.0.1</t>
   </si>
   <si>
-    <t>representant</t>
-  </si>
-  <si>
-    <t>http://helsenorge.no/fhir/StructureDefinition/representant</t>
+    <t>hn-extension-representant</t>
+  </si>
+  <si>
+    <t>http://helsenorge.no/fhir/StructureDefinition/hn-extension-representant</t>
+  </si>
+  <si>
+    <t>HnExtensionRepresentant</t>
   </si>
   <si>
     <t>Representant</t>
   </si>
   <si>
-    <t>Person som representerer en annen etter avtale.</t>
+    <t>Person som representerer en annen etter avtale, vedtakk mm.</t>
   </si>
   <si>
     <t>complex-type</t>
@@ -1351,7 +1354,7 @@
         <v>9</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27">
@@ -1395,7 +1398,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33">
@@ -1423,7 +1426,7 @@
         <v>24</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37">
@@ -1431,7 +1434,7 @@
         <v>26</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38">
@@ -1439,7 +1442,7 @@
         <v>28</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39">
@@ -1460,10 +1463,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1485,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="25.0859375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="38.84375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.84375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="7.015625" customWidth="true" bestFit="true" hidden="true"/>
@@ -6292,10 +6295,10 @@
         <v>279</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6321,10 +6324,10 @@
         <v>38</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
@@ -6375,7 +6378,7 @@
         <v>37</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>35</v>
@@ -6395,10 +6398,10 @@
         <v>279</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C47" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6498,10 +6501,10 @@
         <v>279</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6527,10 +6530,10 @@
         <v>88</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
@@ -6601,13 +6604,13 @@
         <v>279</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D49" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E49" t="s" s="2">
         <v>37</v>
@@ -6632,10 +6635,10 @@
         <v>88</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
@@ -6706,10 +6709,10 @@
         <v>279</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -6809,10 +6812,10 @@
         <v>279</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -6838,10 +6841,10 @@
         <v>88</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
@@ -6912,10 +6915,10 @@
         <v>279</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C52" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -6941,13 +6944,13 @@
         <v>58</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O52" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P52" s="2"/>
       <c r="Q52" t="s" s="2">
@@ -6955,7 +6958,7 @@
       </c>
       <c r="R52" s="2"/>
       <c r="S52" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="T52" t="s" s="2">
         <v>37</v>
@@ -6997,7 +7000,7 @@
         <v>37</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>43</v>
@@ -7017,10 +7020,10 @@
         <v>279</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C53" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7046,10 +7049,10 @@
         <v>115</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -7100,7 +7103,7 @@
         <v>37</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>35</v>
@@ -7120,13 +7123,13 @@
         <v>279</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C54" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D54" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E54" t="s" s="2">
         <v>37</v>
@@ -7151,10 +7154,10 @@
         <v>88</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -7225,10 +7228,10 @@
         <v>279</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C55" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7328,10 +7331,10 @@
         <v>279</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
@@ -7433,10 +7436,10 @@
         <v>279</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C57" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -7462,13 +7465,13 @@
         <v>58</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O57" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P57" s="2"/>
       <c r="Q57" t="s" s="2">
@@ -7476,7 +7479,7 @@
       </c>
       <c r="R57" s="2"/>
       <c r="S57" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="T57" t="s" s="2">
         <v>37</v>
@@ -7518,7 +7521,7 @@
         <v>37</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AH57" t="s" s="2">
         <v>43</v>
@@ -7538,10 +7541,10 @@
         <v>279</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C58" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -7564,13 +7567,13 @@
         <v>37</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -7621,7 +7624,7 @@
         <v>37</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>35</v>
@@ -7641,10 +7644,10 @@
         <v>279</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
@@ -7670,13 +7673,13 @@
         <v>58</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O59" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P59" s="2"/>
       <c r="Q59" t="s" s="2">
@@ -7726,7 +7729,7 @@
         <v>37</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>43</v>
@@ -7746,10 +7749,10 @@
         <v>279</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C60" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -7772,13 +7775,13 @@
         <v>37</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
@@ -7829,7 +7832,7 @@
         <v>37</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>35</v>

</xml_diff>